<commit_message>
SVD - watermarking, extraction
</commit_message>
<xml_diff>
--- a/metrics/FullReference.xlsx
+++ b/metrics/FullReference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Desktop\Watermarking\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDIA_II_SEMESTR\magisterka_v1\Watermarking\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3681BA-8064-4C6B-A10B-8727FD88C7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C587B644-CA2A-4788-BE8E-5211B063CA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7370" activeTab="1" xr2:uid="{A34ABFE7-F0E3-4F6A-9A02-879C9DDFDA35}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{A34ABFE7-F0E3-4F6A-9A02-879C9DDFDA35}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -405,15 +405,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B423D9A-3683-4BB7-92EE-78004B342E21}">
-  <dimension ref="A1:E271"/>
+  <dimension ref="A1:E371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="D271" sqref="D271"/>
+    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="D371" sqref="D371"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31.460353315984801</v>
       </c>
@@ -444,7 +444,7 @@
         <v>0.99229097366333008</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>31.475107014629081</v>
       </c>
@@ -458,7 +458,7 @@
         <v>0.99380135536193848</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>31.457382225535326</v>
       </c>
@@ -472,7 +472,7 @@
         <v>0.99254339933395386</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31.463647889754402</v>
       </c>
@@ -486,7 +486,7 @@
         <v>0.99376237392425537</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>31.458930048618164</v>
       </c>
@@ -500,7 +500,7 @@
         <v>0.97592788934707642</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>31.45895032943762</v>
       </c>
@@ -514,7 +514,7 @@
         <v>0.99298012256622314</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>31.457382225535326</v>
       </c>
@@ -528,7 +528,7 @@
         <v>0.99488461017608643</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31.457415170171458</v>
       </c>
@@ -542,7 +542,7 @@
         <v>0.99547719955444336</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31.45984024363905</v>
       </c>
@@ -556,7 +556,7 @@
         <v>0.99572855234146118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31.476180102086055</v>
       </c>
@@ -570,7 +570,7 @@
         <v>0.99647128582000732</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>31.457382225535326</v>
       </c>
@@ -584,7 +584,7 @@
         <v>0.99355775117874146</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>31.457382225535326</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0.99531573057174683</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>31.457382225535326</v>
       </c>
@@ -612,7 +612,7 @@
         <v>0.99556457996368408</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>31.462955957248006</v>
       </c>
@@ -626,7 +626,7 @@
         <v>0.99162042140960693</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31.457382225535326</v>
       </c>
@@ -640,7 +640,7 @@
         <v>0.993094801902771</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>31.457382225535326</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0.99340355396270752</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31.458193243070248</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0.99528539180755615</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31.459508089089635</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0.99404621124267578</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31.457382225535326</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0.99397420883178711</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31.457382225535326</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.99370265007019043</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>31.46740045568102</v>
       </c>
@@ -724,7 +724,7 @@
         <v>0.99563568830490112</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>31.457382225535326</v>
       </c>
@@ -738,7 +738,7 @@
         <v>0.98834222555160522</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>31.457382225535326</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0.98973780870437622</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>31.457382225535326</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.99360328912734985</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>31.457382225535326</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0.99422210454940796</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>31.457382225535326</v>
       </c>
@@ -794,7 +794,7 @@
         <v>0.99119067192077637</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>31.457382225535326</v>
       </c>
@@ -808,7 +808,7 @@
         <v>0.98585397005081177</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31.511009425675777</v>
       </c>
@@ -822,7 +822,7 @@
         <v>0.99031245708465576</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>31.459874052142304</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.98276042938232422</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31.457382225535326</v>
       </c>
@@ -850,7 +850,7 @@
         <v>0.99024671316146851</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31.457382225535326</v>
       </c>
@@ -864,7 +864,7 @@
         <v>0.97785604000091553</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31.457382225535326</v>
       </c>
@@ -878,7 +878,7 @@
         <v>0.97127777338027954</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31.457382225535326</v>
       </c>
@@ -892,7 +892,7 @@
         <v>0.98167824745178223</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31.457748854288337</v>
       </c>
@@ -906,7 +906,7 @@
         <v>0.98901033401489258</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>31.457382225535326</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0.99412769079208374</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31.457382225535326</v>
       </c>
@@ -934,7 +934,7 @@
         <v>0.98018062114715576</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>31.48217900443116</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0.98626071214675903</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>31.594161283427976</v>
       </c>
@@ -962,7 +962,7 @@
         <v>0.9901924729347229</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>31.457382225535326</v>
       </c>
@@ -976,7 +976,7 @@
         <v>0.98771649599075317</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>31.457382225535326</v>
       </c>
@@ -990,7 +990,7 @@
         <v>0.99129021167755127</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>31.457389828121482</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0.97205287218093872</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>31.457382225535326</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>0.99162399768829346</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>31.457382225535326</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0.98556065559387207</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>31.457382225535326</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>0.98771345615386963</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>31.459243566869802</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>0.98591864109039307</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>31.457382225535326</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>0.98888099193572998</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>31.45798118115426</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>0.99364262819290161</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>31.457382225535326</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>0.9896579384803772</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>31.457382225535326</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>0.99333339929580688</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>31.481292995405582</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>0.9934116005897522</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>31.482591064452023</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0.99446415901184082</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>31.457382225535326</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>0.97234445810317993</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>31.457382225535326</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>0.99471521377563477</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>31.457382225535326</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>0.9765547513961792</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>31.457382225535326</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>0.96343278884887695</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>31.457382225535326</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>0.9928707480430603</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>31.457382225535326</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>0.98264777660369873</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>31.457382225535326</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>0.98510146141052246</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>31.457382225535326</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>0.98962223529815674</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>31.457382225535326</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>0.98841941356658936</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>31.457382225535326</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>0.99002617597579956</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>31.457486973449427</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>0.97207307815551758</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>31.776495590210871</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>0.9896886944770813</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>31.554431826691459</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>0.99438005685806274</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>31.483088137326646</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>0.99208211898803711</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>31.457394896519652</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>0.99036258459091187</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>31.457382225535326</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>0.99475568532943726</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>31.457382225535326</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>0.99188506603240967</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>31.458499103592739</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0.972930908203125</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>31.457382225535326</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0.98611551523208618</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>31.457382225535326</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0.99353116750717163</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>31.457920352555611</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>0.99475717544555664</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>31.457407567540937</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>0.9921259880065918</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>31.457382225535326</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>0.99102997779846191</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>31.482015890440998</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>0.99230664968490601</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>31.457382225535326</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0.99017351865768433</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>31.466893322823914</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>0.99613142013549805</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>31.457382225535326</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>0.98819714784622192</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>31.457382225535326</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>0.98251873254776001</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>31.478325375137999</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>0.98958951234817505</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>31.457382225535326</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0.9948112964630127</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>31.459959419784312</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>0.99432623386383057</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>31.457382225535326</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>0.99312800168991089</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>31.457382225535326</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0.98906868696212769</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>31.457382225535326</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0.99289190769195557</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>31.457382225535326</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>0.9894828200340271</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>31.457382225535326</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>0.9899713397026062</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>31.457382225535326</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>0.9927600622177124</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>31.457382225535326</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0.99038112163543701</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>31.457382225535326</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0.98876792192459106</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>31.457382225535326</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0.9874146580696106</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>31.457382225535326</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0.98846215009689331</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>31.457382225535326</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>0.98876059055328369</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>31.457382225535326</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0.98941034078598022</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>31.457382225535326</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>0.99363517761230469</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>31.457524987430151</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>0.98390841484069824</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>31.538008007584928</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0.97709882259368896</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>31.457382225535326</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0.98631662130355835</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>31.457382225535326</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>0.99362462759017944</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>31.457382225535326</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0.99234211444854736</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>31.460353315984801</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>0.99229097366333008</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>31.475107014629081</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>0.99380135536193848</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>31.457382225535326</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>0.99254339933395386</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>31.463647889754402</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>0.99376237392425537</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>31.458930048618164</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.97592788934707642</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>31.45895032943762</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.99298012256622314</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>31.457382225535326</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0.99488461017608643</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>31.457415170171458</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>0.99547719955444336</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>31.45984024363905</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>0.99572855234146118</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>31.476180102086055</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>0.99647128582000732</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>31.457382225535326</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0.99355775117874146</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>31.457382225535326</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>0.99531573057174683</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>31.457382225535326</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0.99556457996368408</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>31.462955957248006</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>0.99162042140960693</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>31.457382225535326</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0.993094801902771</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>31.457382225535326</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>0.99340355396270752</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>31.458193243070248</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0.99528539180755615</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>31.459508089089635</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>0.99404621124267578</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>31.457382225535326</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>0.99397420883178711</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>31.457382225535326</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.99370265007019043</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>31.46740045568102</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>0.99563568830490112</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>31.457382225535326</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0.98834222555160522</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>31.457382225535326</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0.98973780870437622</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>31.457382225535326</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0.99360328912734985</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>31.457382225535326</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0.99422210454940796</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>31.457382225535326</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>0.99119067192077637</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>31.457382225535326</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0.98585397005081177</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>31.511009425675777</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0.99031245708465576</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>31.459874052142304</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>0.98276042938232422</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>31.457382225535326</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>0.99024671316146851</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>31.457382225535326</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.97785604000091553</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>31.457382225535326</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0.97127777338027954</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>31.457382225535326</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>0.98167824745178223</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>31.457748854288337</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>0.98901033401489258</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>31.457382225535326</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>0.99412769079208374</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>31.457382225535326</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0.98018062114715576</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>31.48217900443116</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>0.98626071214675903</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>31.594161283427976</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>0.9901924729347229</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>31.457382225535326</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0.98771649599075317</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>31.457382225535326</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.99129021167755127</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>31.457389828121482</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>0.97205287218093872</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>31.457382225535326</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>0.99162399768829346</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>31.457382225535326</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>0.98556065559387207</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>31.457382225535326</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0.98771345615386963</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>31.459243566869802</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0.98591864109039307</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>31.457382225535326</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>0.98888099193572998</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>31.45798118115426</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0.99364262819290161</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>31.457382225535326</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>0.9896579384803772</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>31.457382225535326</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0.99333339929580688</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>31.481292995405582</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0.9934116005897522</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>31.482591064452023</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>0.99446415901184082</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>31.457382225535326</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>0.97234445810317993</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>31.457382225535326</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>0.99471521377563477</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>31.457382225535326</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0.9765547513961792</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>31.457382225535326</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>0.96343278884887695</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>31.457382225535326</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>0.9928707480430603</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>31.457382225535326</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0.98264777660369873</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>31.457382225535326</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0.98510146141052246</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>31.457382225535326</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>0.98962223529815674</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>31.457382225535326</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>0.98841941356658936</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>31.457382225535326</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0.99002617597579956</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>31.457486973449427</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>0.97207307815551758</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>31.776495590210871</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>0.9896886944770813</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>31.554431826691459</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0.99438005685806274</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>31.483088137326646</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0.99208211898803711</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>31.457394896519652</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>0.99036258459091187</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>31.457382225535326</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>0.99475568532943726</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>31.457382225535326</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>0.99188506603240967</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>31.458499103592739</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>0.972930908203125</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>31.457382225535326</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0.98611551523208618</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>31.457382225535326</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0.99353116750717163</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>31.457920352555611</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0.99475717544555664</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>31.457407567540937</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>0.9921259880065918</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>31.457382225535326</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0.99102997779846191</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>31.482015890440998</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>0.99230664968490601</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>31.457382225535326</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0.99017351865768433</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>31.466893322823914</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>0.99613142013549805</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>31.457382225535326</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>0.98819714784622192</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>31.457382225535326</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0.98251873254776001</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>31.478325375137999</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>0.98958951234817505</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>31.457382225535326</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>0.9948112964630127</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>31.459959419784312</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>0.99432623386383057</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>31.457382225535326</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0.99312800168991089</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>31.457382225535326</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0.98906868696212769</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>31.457382225535326</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>0.99289190769195557</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>31.457382225535326</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0.9894828200340271</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>31.457382225535326</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>0.9899713397026062</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>31.457382225535326</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>0.9927600622177124</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>31.457382225535326</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>0.99038112163543701</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>31.457382225535326</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0.98876792192459106</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>31.457382225535326</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0.9874146580696106</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>31.457382225535326</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0.98846215009689331</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>31.457382225535326</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>0.98876059055328369</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>31.457382225535326</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>0.98941034078598022</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>31.457382225535326</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>0.99363517761230469</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>31.457524987430151</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0.98390841484069824</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>31.538008007584928</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0.97709882259368896</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>31.457382225535326</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>0.98631662130355835</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>31.457382225535326</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>0.99362462759017944</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>31.457382225535326</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>0.99234211444854736</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>31.460353315984801</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>0.99229097366333008</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>31.475107014629081</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0.99380135536193848</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>31.457382225535326</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>0.99254339933395386</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>31.463647889754402</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>0.99376237392425537</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>31.458930048618164</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>0.97592788934707642</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>31.45895032943762</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>0.99298012256622314</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>31.457382225535326</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>0.99488461017608643</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>31.457415170171458</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>0.99547719955444336</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>31.45984024363905</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>0.99572855234146118</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>31.476180102086055</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>0.99647128582000732</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>31.457382225535326</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>0.99355775117874146</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>31.457382225535326</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>0.99531573057174683</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>31.457382225535326</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.99556457996368408</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>31.462955957248006</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>0.99162042140960693</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>31.457382225535326</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>0.993094801902771</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>31.457382225535326</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>0.99340355396270752</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>31.458193243070248</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>0.99528539180755615</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>31.459508089089635</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>0.99404621124267578</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>31.457382225535326</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>0.99397420883178711</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>31.457382225535326</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>0.99370265007019043</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>31.46740045568102</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>0.99563568830490112</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>31.457382225535326</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0.98834222555160522</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>31.457382225535326</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>0.98973780870437622</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>31.457382225535326</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>0.99360328912734985</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>31.457382225535326</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>0.99422210454940796</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>31.457382225535326</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>0.99119067192077637</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>31.457382225535326</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0.98585397005081177</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>31.511009425675777</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>0.99031245708465576</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>31.459874052142304</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>0.98276042938232422</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>31.457382225535326</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>0.99024671316146851</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>31.457382225535326</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>0.97785604000091553</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>31.457382225535326</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>0.97127777338027954</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>31.457382225535326</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>0.98167824745178223</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>31.457748854288337</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>0.98901033401489258</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>31.457382225535326</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0.99412769079208374</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>31.457382225535326</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>0.98018062114715576</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>31.48217900443116</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>0.98626071214675903</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>31.594161283427976</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>0.9901924729347229</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>31.457382225535326</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>0.98771649599075317</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>31.457382225535326</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>0.99129021167755127</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>31.457389828121482</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>0.97205287218093872</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>31.457382225535326</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0.99162399768829346</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>31.457382225535326</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>0.98556065559387207</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>31.457382225535326</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>0.98771345615386963</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>31.459243566869802</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>0.98591864109039307</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>31.457382225535326</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>0.98888099193572998</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>31.45798118115426</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>0.99364262819290161</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>31.457382225535326</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>0.9896579384803772</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>31.457382225535326</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>0.99333339929580688</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>31.481292995405582</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>0.9934116005897522</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>31.482591064452023</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>0.99446415901184082</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>31.457382225535326</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>0.97234445810317993</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>31.457382225535326</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>0.99471521377563477</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>31.457382225535326</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>0.9765547513961792</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>31.457382225535326</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>0.96343278884887695</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>31.457382225535326</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>0.9928707480430603</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>31.457382225535326</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>0.98264777660369873</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>31.457382225535326</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>0.98510146141052246</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>31.457382225535326</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>0.98962223529815674</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>31.457382225535326</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>0.98841941356658936</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>31.457382225535326</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>0.99002617597579956</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>31.457486973449427</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0.97207307815551758</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>31.776495590210871</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>0.9896886944770813</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>31.554431826691459</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>0.99438005685806274</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>31.483088137326646</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>0.99208211898803711</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>31.457394896519652</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>0.99036258459091187</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>31.457382225535326</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>0.99475568532943726</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>31.457382225535326</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>0.99188506603240967</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>31.458499103592739</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>0.972930908203125</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>31.457382225535326</v>
       </c>
@@ -4208,6 +4208,1406 @@
       </c>
       <c r="D271">
         <v>0.98611551523208618</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>30.884991819531248</v>
+      </c>
+      <c r="B272">
+        <v>0.93787670146945645</v>
+      </c>
+      <c r="C272">
+        <v>0.97494691610336304</v>
+      </c>
+      <c r="D272">
+        <v>0.97734105587005615</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>30.232177231764986</v>
+      </c>
+      <c r="B273">
+        <v>0.95600711929387705</v>
+      </c>
+      <c r="C273">
+        <v>0.97843945026397705</v>
+      </c>
+      <c r="D273">
+        <v>0.97936242818832397</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>29.225598088941478</v>
+      </c>
+      <c r="B274">
+        <v>0.92110990375667168</v>
+      </c>
+      <c r="C274">
+        <v>0.9623638391494751</v>
+      </c>
+      <c r="D274">
+        <v>0.96708589792251587</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>31.491375112494303</v>
+      </c>
+      <c r="B275">
+        <v>0.94827508567445296</v>
+      </c>
+      <c r="C275">
+        <v>0.98608797788619995</v>
+      </c>
+      <c r="D275">
+        <v>0.98707765340805054</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>29.764346023978341</v>
+      </c>
+      <c r="B276">
+        <v>0.91024014274455756</v>
+      </c>
+      <c r="C276">
+        <v>0.97129684686660767</v>
+      </c>
+      <c r="D276">
+        <v>0.9726906418800354</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>30.838911893093645</v>
+      </c>
+      <c r="B277">
+        <v>0.96572722183461301</v>
+      </c>
+      <c r="C277">
+        <v>0.9851539134979248</v>
+      </c>
+      <c r="D277">
+        <v>0.98551338911056519</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>28.905887746538966</v>
+      </c>
+      <c r="B278">
+        <v>0.95795551089755315</v>
+      </c>
+      <c r="C278">
+        <v>0.96270757913589478</v>
+      </c>
+      <c r="D278">
+        <v>0.96306413412094116</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>28.019119571019399</v>
+      </c>
+      <c r="B279">
+        <v>0.94807078916661269</v>
+      </c>
+      <c r="C279">
+        <v>0.95676916837692261</v>
+      </c>
+      <c r="D279">
+        <v>0.95879405736923218</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>28.77038559817569</v>
+      </c>
+      <c r="B280">
+        <v>0.96308982238295593</v>
+      </c>
+      <c r="C280">
+        <v>0.95873183012008667</v>
+      </c>
+      <c r="D280">
+        <v>0.96091490983963013</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>30.160446436326794</v>
+      </c>
+      <c r="B281">
+        <v>0.98653480280957728</v>
+      </c>
+      <c r="C281">
+        <v>0.98045176267623901</v>
+      </c>
+      <c r="D281">
+        <v>0.98221975564956665</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>27.192974788612329</v>
+      </c>
+      <c r="B282">
+        <v>0.9636226904717875</v>
+      </c>
+      <c r="C282">
+        <v>0.94199216365814209</v>
+      </c>
+      <c r="D282">
+        <v>0.95054060220718384</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>29.108049584328342</v>
+      </c>
+      <c r="B283">
+        <v>0.96890461463707012</v>
+      </c>
+      <c r="C283">
+        <v>0.96930146217346191</v>
+      </c>
+      <c r="D283">
+        <v>0.97204148769378662</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>26.488880574944279</v>
+      </c>
+      <c r="B284">
+        <v>0.94804556648125482</v>
+      </c>
+      <c r="C284">
+        <v>0.92666256427764893</v>
+      </c>
+      <c r="D284">
+        <v>0.93288177251815796</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>28.877743977659073</v>
+      </c>
+      <c r="B285">
+        <v>0.88955376340308601</v>
+      </c>
+      <c r="C285">
+        <v>0.95870190858840942</v>
+      </c>
+      <c r="D285">
+        <v>0.96118825674057007</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>28.642999517895969</v>
+      </c>
+      <c r="B286">
+        <v>0.97164980554689029</v>
+      </c>
+      <c r="C286">
+        <v>0.96244931221008301</v>
+      </c>
+      <c r="D286">
+        <v>0.96829360723495483</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>27.417205253527278</v>
+      </c>
+      <c r="B287">
+        <v>0.94758102199169869</v>
+      </c>
+      <c r="C287">
+        <v>0.91374129056930542</v>
+      </c>
+      <c r="D287">
+        <v>0.92621058225631714</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>28.005678257361176</v>
+      </c>
+      <c r="B288">
+        <v>0.9650479329497762</v>
+      </c>
+      <c r="C288">
+        <v>0.95276808738708496</v>
+      </c>
+      <c r="D288">
+        <v>0.9571683406829834</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>29.453823975891872</v>
+      </c>
+      <c r="B289">
+        <v>0.9347752651936817</v>
+      </c>
+      <c r="C289">
+        <v>0.9651067852973938</v>
+      </c>
+      <c r="D289">
+        <v>0.96731925010681152</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>28.843284278140228</v>
+      </c>
+      <c r="B290">
+        <v>0.97310080569553514</v>
+      </c>
+      <c r="C290">
+        <v>0.96422672271728516</v>
+      </c>
+      <c r="D290">
+        <v>0.96810626983642578</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>28.316695010280984</v>
+      </c>
+      <c r="B291">
+        <v>0.97345233722350788</v>
+      </c>
+      <c r="C291">
+        <v>0.95797502994537354</v>
+      </c>
+      <c r="D291">
+        <v>0.9644085168838501</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>30.578404202653537</v>
+      </c>
+      <c r="B292">
+        <v>0.97312897720959124</v>
+      </c>
+      <c r="C292">
+        <v>0.98169988393783569</v>
+      </c>
+      <c r="D292">
+        <v>0.98322415351867676</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>28.692042977452136</v>
+      </c>
+      <c r="B293">
+        <v>0.95454488517181613</v>
+      </c>
+      <c r="C293">
+        <v>0.96613532304763794</v>
+      </c>
+      <c r="D293">
+        <v>0.9697994589805603</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>28.810784223790424</v>
+      </c>
+      <c r="B294">
+        <v>0.93301095103475329</v>
+      </c>
+      <c r="C294">
+        <v>0.95973515510559082</v>
+      </c>
+      <c r="D294">
+        <v>0.96624445915222168</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>26.256595349498294</v>
+      </c>
+      <c r="B295">
+        <v>0.90202193570765343</v>
+      </c>
+      <c r="C295">
+        <v>0.92141246795654297</v>
+      </c>
+      <c r="D295">
+        <v>0.92901331186294556</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>28.298897117481513</v>
+      </c>
+      <c r="B296">
+        <v>0.90654302447610169</v>
+      </c>
+      <c r="C296">
+        <v>0.95005124807357788</v>
+      </c>
+      <c r="D296">
+        <v>0.9546477198600769</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>29.013004679475749</v>
+      </c>
+      <c r="B297">
+        <v>0.93795229212206532</v>
+      </c>
+      <c r="C297">
+        <v>0.96180248260498047</v>
+      </c>
+      <c r="D297">
+        <v>0.96588134765625</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>27.630911229603292</v>
+      </c>
+      <c r="B298">
+        <v>0.92074707731479122</v>
+      </c>
+      <c r="C298">
+        <v>0.95217907428741455</v>
+      </c>
+      <c r="D298">
+        <v>0.95720416307449341</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>31.278478109127555</v>
+      </c>
+      <c r="B299">
+        <v>0.96164221372779646</v>
+      </c>
+      <c r="C299">
+        <v>0.98643571138381958</v>
+      </c>
+      <c r="D299">
+        <v>0.98604041337966919</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>31.458586134142092</v>
+      </c>
+      <c r="B300">
+        <v>0.93725983229310772</v>
+      </c>
+      <c r="C300">
+        <v>0.9620634913444519</v>
+      </c>
+      <c r="D300">
+        <v>0.96842259168624878</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>29.259542331831639</v>
+      </c>
+      <c r="B301">
+        <v>0.86810778368255115</v>
+      </c>
+      <c r="C301">
+        <v>0.96081727743148804</v>
+      </c>
+      <c r="D301">
+        <v>0.96466118097305298</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>30.717688749998416</v>
+      </c>
+      <c r="B302">
+        <v>0.91070448935421189</v>
+      </c>
+      <c r="C302">
+        <v>0.97301310300827026</v>
+      </c>
+      <c r="D302">
+        <v>0.97581422328948975</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>28.690315708289901</v>
+      </c>
+      <c r="B303">
+        <v>0.94151979061060287</v>
+      </c>
+      <c r="C303">
+        <v>0.96231842041015625</v>
+      </c>
+      <c r="D303">
+        <v>0.96425068378448486</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>28.455570814245821</v>
+      </c>
+      <c r="B304">
+        <v>0.85137890009457606</v>
+      </c>
+      <c r="C304">
+        <v>0.95751041173934937</v>
+      </c>
+      <c r="D304">
+        <v>0.96026158332824707</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>28.79816420054231</v>
+      </c>
+      <c r="B305">
+        <v>0.95547786720252192</v>
+      </c>
+      <c r="C305">
+        <v>0.96637201309204102</v>
+      </c>
+      <c r="D305">
+        <v>0.96787542104721069</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>30.094777484125061</v>
+      </c>
+      <c r="B306">
+        <v>0.97161536890653588</v>
+      </c>
+      <c r="C306">
+        <v>0.962455153465271</v>
+      </c>
+      <c r="D306">
+        <v>0.9680294394493103</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>27.791408751903393</v>
+      </c>
+      <c r="B307">
+        <v>0.86726693597985771</v>
+      </c>
+      <c r="C307">
+        <v>0.94819879531860352</v>
+      </c>
+      <c r="D307">
+        <v>0.95223760604858398</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>28.880828882109533</v>
+      </c>
+      <c r="B308">
+        <v>0.88217851099647238</v>
+      </c>
+      <c r="C308">
+        <v>0.96263974905014038</v>
+      </c>
+      <c r="D308">
+        <v>0.9646955132484436</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>31.534328092387934</v>
+      </c>
+      <c r="B309">
+        <v>0.9575402389805423</v>
+      </c>
+      <c r="C309">
+        <v>0.98585832118988037</v>
+      </c>
+      <c r="D309">
+        <v>0.98599535226821899</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>29.777095703881379</v>
+      </c>
+      <c r="B310">
+        <v>0.91709382883880153</v>
+      </c>
+      <c r="C310">
+        <v>0.97224634885787964</v>
+      </c>
+      <c r="D310">
+        <v>0.97554546594619751</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>25.016929953640453</v>
+      </c>
+      <c r="B311">
+        <v>0.88842911049275275</v>
+      </c>
+      <c r="C311">
+        <v>0.89223074913024902</v>
+      </c>
+      <c r="D311">
+        <v>0.9049457311630249</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>29.485618443291614</v>
+      </c>
+      <c r="B312">
+        <v>0.87924375575429348</v>
+      </c>
+      <c r="C312">
+        <v>0.96865785121917725</v>
+      </c>
+      <c r="D312">
+        <v>0.97070884704589844</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>28.205857959398912</v>
+      </c>
+      <c r="B313">
+        <v>0.92408196780464236</v>
+      </c>
+      <c r="C313">
+        <v>0.94119834899902344</v>
+      </c>
+      <c r="D313">
+        <v>0.94621783494949341</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>27.467901675947047</v>
+      </c>
+      <c r="B314">
+        <v>0.88672983611159339</v>
+      </c>
+      <c r="C314">
+        <v>0.93069666624069214</v>
+      </c>
+      <c r="D314">
+        <v>0.940818190574646</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>27.167301642523434</v>
+      </c>
+      <c r="B315">
+        <v>0.83036664255649983</v>
+      </c>
+      <c r="C315">
+        <v>0.93591952323913574</v>
+      </c>
+      <c r="D315">
+        <v>0.94228446483612061</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>28.914381427821567</v>
+      </c>
+      <c r="B316">
+        <v>0.96009983088621365</v>
+      </c>
+      <c r="C316">
+        <v>0.96652531623840332</v>
+      </c>
+      <c r="D316">
+        <v>0.97203207015991211</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>26.246706012418272</v>
+      </c>
+      <c r="B317">
+        <v>0.92361272051957521</v>
+      </c>
+      <c r="C317">
+        <v>0.88641637563705444</v>
+      </c>
+      <c r="D317">
+        <v>0.90668016672134399</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>32.378547306794609</v>
+      </c>
+      <c r="B318">
+        <v>0.93397511579993719</v>
+      </c>
+      <c r="C318">
+        <v>0.98799037933349609</v>
+      </c>
+      <c r="D318">
+        <v>0.98844796419143677</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>26.283267185496157</v>
+      </c>
+      <c r="B319">
+        <v>0.89517160949500718</v>
+      </c>
+      <c r="C319">
+        <v>0.88536489009857178</v>
+      </c>
+      <c r="D319">
+        <v>0.9060102105140686</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>27.973913401456048</v>
+      </c>
+      <c r="B320">
+        <v>0.9562522374119129</v>
+      </c>
+      <c r="C320">
+        <v>0.96221661567687988</v>
+      </c>
+      <c r="D320">
+        <v>0.9671667218208313</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>28.948253517262579</v>
+      </c>
+      <c r="B321">
+        <v>0.96684925759368723</v>
+      </c>
+      <c r="C321">
+        <v>0.96613317728042603</v>
+      </c>
+      <c r="D321">
+        <v>0.96994614601135254</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>29.230528467152084</v>
+      </c>
+      <c r="B322">
+        <v>0.96363763318400308</v>
+      </c>
+      <c r="C322">
+        <v>0.96810787916183472</v>
+      </c>
+      <c r="D322">
+        <v>0.97038781642913818</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>29.389065100464524</v>
+      </c>
+      <c r="B323">
+        <v>0.88023604256726817</v>
+      </c>
+      <c r="C323">
+        <v>0.95091444253921509</v>
+      </c>
+      <c r="D323">
+        <v>0.95705443620681763</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>30.76896400773947</v>
+      </c>
+      <c r="B324">
+        <v>0.96808562639602225</v>
+      </c>
+      <c r="C324">
+        <v>0.98024886846542358</v>
+      </c>
+      <c r="D324">
+        <v>0.98258751630783081</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>28.154295891047724</v>
+      </c>
+      <c r="B325">
+        <v>0.89009846061048781</v>
+      </c>
+      <c r="C325">
+        <v>0.95698988437652588</v>
+      </c>
+      <c r="D325">
+        <v>0.95925235748291016</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>27.277957974066183</v>
+      </c>
+      <c r="B326">
+        <v>0.91722159368001777</v>
+      </c>
+      <c r="C326">
+        <v>0.95490407943725586</v>
+      </c>
+      <c r="D326">
+        <v>0.95679992437362671</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>29.657892538063166</v>
+      </c>
+      <c r="B327">
+        <v>0.91656738136324822</v>
+      </c>
+      <c r="C327">
+        <v>0.97279840707778931</v>
+      </c>
+      <c r="D327">
+        <v>0.97529137134552002</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>29.005497529450945</v>
+      </c>
+      <c r="B328">
+        <v>0.8245078498406625</v>
+      </c>
+      <c r="C328">
+        <v>0.93930613994598389</v>
+      </c>
+      <c r="D328">
+        <v>0.95141661167144775</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>30.03109693245538</v>
+      </c>
+      <c r="B329">
+        <v>0.86469153261816045</v>
+      </c>
+      <c r="C329">
+        <v>0.96335941553115845</v>
+      </c>
+      <c r="D329">
+        <v>0.96693074703216553</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>27.146604533317728</v>
+      </c>
+      <c r="B330">
+        <v>0.89400861315137536</v>
+      </c>
+      <c r="C330">
+        <v>0.9311983585357666</v>
+      </c>
+      <c r="D330">
+        <v>0.94108682870864868</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>26.472487942499505</v>
+      </c>
+      <c r="B331">
+        <v>0.91216011695355081</v>
+      </c>
+      <c r="C331">
+        <v>0.94553226232528687</v>
+      </c>
+      <c r="D331">
+        <v>0.95031642913818359</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>26.1301687999485</v>
+      </c>
+      <c r="B332">
+        <v>0.86548804686957226</v>
+      </c>
+      <c r="C332">
+        <v>0.89816039800643921</v>
+      </c>
+      <c r="D332">
+        <v>0.9085121750831604</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>29.816000370478442</v>
+      </c>
+      <c r="B333">
+        <v>0.90580574145919934</v>
+      </c>
+      <c r="C333">
+        <v>0.98132234811782837</v>
+      </c>
+      <c r="D333">
+        <v>0.98259764909744263</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>29.537032287763957</v>
+      </c>
+      <c r="B334">
+        <v>0.9366923693656467</v>
+      </c>
+      <c r="C334">
+        <v>0.97076570987701416</v>
+      </c>
+      <c r="D334">
+        <v>0.97153741121292114</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>27.63273617691484</v>
+      </c>
+      <c r="B335">
+        <v>0.9559153788512128</v>
+      </c>
+      <c r="C335">
+        <v>0.94664245843887329</v>
+      </c>
+      <c r="D335">
+        <v>0.95211249589920044</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>29.242172339735614</v>
+      </c>
+      <c r="B336">
+        <v>0.931035249694108</v>
+      </c>
+      <c r="C336">
+        <v>0.97268128395080566</v>
+      </c>
+      <c r="D336">
+        <v>0.97408711910247803</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>29.542585438418143</v>
+      </c>
+      <c r="B337">
+        <v>0.87443598722811255</v>
+      </c>
+      <c r="C337">
+        <v>0.97885227203369141</v>
+      </c>
+      <c r="D337">
+        <v>0.98033875226974487</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>28.313654813982353</v>
+      </c>
+      <c r="B338">
+        <v>0.9415853735917824</v>
+      </c>
+      <c r="C338">
+        <v>0.9469800591468811</v>
+      </c>
+      <c r="D338">
+        <v>0.95432603359222412</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>27.501418632592344</v>
+      </c>
+      <c r="B339">
+        <v>0.90772575744414552</v>
+      </c>
+      <c r="C339">
+        <v>0.94968301057815552</v>
+      </c>
+      <c r="D339">
+        <v>0.95690619945526123</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>32.968268658860595</v>
+      </c>
+      <c r="B340">
+        <v>0.89648471819168307</v>
+      </c>
+      <c r="C340">
+        <v>0.97740107774734497</v>
+      </c>
+      <c r="D340">
+        <v>0.97861534357070923</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>25.322038756809498</v>
+      </c>
+      <c r="B341">
+        <v>0.91927180455145985</v>
+      </c>
+      <c r="C341">
+        <v>0.90668016672134399</v>
+      </c>
+      <c r="D341">
+        <v>0.92211461067199707</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>30.186733578485047</v>
+      </c>
+      <c r="B342">
+        <v>0.91637823880447944</v>
+      </c>
+      <c r="C342">
+        <v>0.96924275159835815</v>
+      </c>
+      <c r="D342">
+        <v>0.97205644845962524</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>28.63144359599325</v>
+      </c>
+      <c r="B343">
+        <v>0.96344589526371038</v>
+      </c>
+      <c r="C343">
+        <v>0.95947086811065674</v>
+      </c>
+      <c r="D343">
+        <v>0.96272373199462891</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>27.016604128835795</v>
+      </c>
+      <c r="B344">
+        <v>0.91974266345077871</v>
+      </c>
+      <c r="C344">
+        <v>0.94197505712509155</v>
+      </c>
+      <c r="D344">
+        <v>0.94905740022659302</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>29.117391950880034</v>
+      </c>
+      <c r="B345">
+        <v>0.90211528293746468</v>
+      </c>
+      <c r="C345">
+        <v>0.94567298889160156</v>
+      </c>
+      <c r="D345">
+        <v>0.95354980230331421</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>29.699927650793988</v>
+      </c>
+      <c r="B346">
+        <v>0.94280811030913148</v>
+      </c>
+      <c r="C346">
+        <v>0.9703221321105957</v>
+      </c>
+      <c r="D346">
+        <v>0.97310072183609009</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>28.044199793217572</v>
+      </c>
+      <c r="B347">
+        <v>0.90933526524086672</v>
+      </c>
+      <c r="C347">
+        <v>0.94339448213577271</v>
+      </c>
+      <c r="D347">
+        <v>0.94398403167724609</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>27.055280184160303</v>
+      </c>
+      <c r="B348">
+        <v>0.95213175848002762</v>
+      </c>
+      <c r="C348">
+        <v>0.94708359241485596</v>
+      </c>
+      <c r="D348">
+        <v>0.94651997089385986</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>29.329601267632377</v>
+      </c>
+      <c r="B349">
+        <v>0.92617573393499331</v>
+      </c>
+      <c r="C349">
+        <v>0.95577549934387207</v>
+      </c>
+      <c r="D349">
+        <v>0.96071159839630127</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>26.728381790460929</v>
+      </c>
+      <c r="B350">
+        <v>0.87935009790469454</v>
+      </c>
+      <c r="C350">
+        <v>0.92927467823028564</v>
+      </c>
+      <c r="D350">
+        <v>0.93047761917114258</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>28.568540631665286</v>
+      </c>
+      <c r="B351">
+        <v>0.91831523301824258</v>
+      </c>
+      <c r="C351">
+        <v>0.96863031387329102</v>
+      </c>
+      <c r="D351">
+        <v>0.97022879123687744</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>30.29240509551968</v>
+      </c>
+      <c r="B352">
+        <v>0.9511456216794163</v>
+      </c>
+      <c r="C352">
+        <v>0.97640013694763184</v>
+      </c>
+      <c r="D352">
+        <v>0.97879302501678467</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>29.975902762929834</v>
+      </c>
+      <c r="B353">
+        <v>0.96179739086438198</v>
+      </c>
+      <c r="C353">
+        <v>0.97165036201477051</v>
+      </c>
+      <c r="D353">
+        <v>0.97467690706253052</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>28.904032493885676</v>
+      </c>
+      <c r="B354">
+        <v>0.96529694157535584</v>
+      </c>
+      <c r="C354">
+        <v>0.96530157327651978</v>
+      </c>
+      <c r="D354">
+        <v>0.96986854076385498</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>28.13982621870619</v>
+      </c>
+      <c r="B355">
+        <v>0.91057628149817615</v>
+      </c>
+      <c r="C355">
+        <v>0.95816075801849365</v>
+      </c>
+      <c r="D355">
+        <v>0.96348714828491211</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>27.622503558945596</v>
+      </c>
+      <c r="B356">
+        <v>0.94188005272309205</v>
+      </c>
+      <c r="C356">
+        <v>0.94920414686203003</v>
+      </c>
+      <c r="D356">
+        <v>0.95552200078964233</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>29.636398073427976</v>
+      </c>
+      <c r="B357">
+        <v>0.9230685834337431</v>
+      </c>
+      <c r="C357">
+        <v>0.96576213836669922</v>
+      </c>
+      <c r="D357">
+        <v>0.96748369932174683</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>29.296936457275706</v>
+      </c>
+      <c r="B358">
+        <v>0.94250797858666358</v>
+      </c>
+      <c r="C358">
+        <v>0.96999663114547729</v>
+      </c>
+      <c r="D358">
+        <v>0.97424274682998657</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>27.429437456839413</v>
+      </c>
+      <c r="B359">
+        <v>0.94625754531001494</v>
+      </c>
+      <c r="C359">
+        <v>0.94413894414901733</v>
+      </c>
+      <c r="D359">
+        <v>0.95154678821563721</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>26.876318360865248</v>
+      </c>
+      <c r="B360">
+        <v>0.90616082612139137</v>
+      </c>
+      <c r="C360">
+        <v>0.91937398910522461</v>
+      </c>
+      <c r="D360">
+        <v>0.93156582117080688</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>26.929002301253753</v>
+      </c>
+      <c r="B361">
+        <v>0.91517160768026651</v>
+      </c>
+      <c r="C361">
+        <v>0.9096294641494751</v>
+      </c>
+      <c r="D361">
+        <v>0.92292696237564087</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>26.70810492242915</v>
+      </c>
+      <c r="B362">
+        <v>0.88591202977613248</v>
+      </c>
+      <c r="C362">
+        <v>0.91720706224441528</v>
+      </c>
+      <c r="D362">
+        <v>0.92887097597122192</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>26.654656431454985</v>
+      </c>
+      <c r="B363">
+        <v>0.92373921258347236</v>
+      </c>
+      <c r="C363">
+        <v>0.93801069259643555</v>
+      </c>
+      <c r="D363">
+        <v>0.9444548487663269</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>27.694606121307757</v>
+      </c>
+      <c r="B364">
+        <v>0.89405064516060717</v>
+      </c>
+      <c r="C364">
+        <v>0.95072108507156372</v>
+      </c>
+      <c r="D364">
+        <v>0.95877426862716675</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>28.868894743899389</v>
+      </c>
+      <c r="B365">
+        <v>0.92844747342693079</v>
+      </c>
+      <c r="C365">
+        <v>0.96965295076370239</v>
+      </c>
+      <c r="D365">
+        <v>0.97270709276199341</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>27.978165621540789</v>
+      </c>
+      <c r="B366">
+        <v>0.93213803883251967</v>
+      </c>
+      <c r="C366">
+        <v>0.94040888547897339</v>
+      </c>
+      <c r="D366">
+        <v>0.94715160131454468</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>32.060230675912067</v>
+      </c>
+      <c r="B367">
+        <v>0.96265908292635571</v>
+      </c>
+      <c r="C367">
+        <v>0.98924672603607178</v>
+      </c>
+      <c r="D367">
+        <v>0.98922693729400635</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>29.436829958998118</v>
+      </c>
+      <c r="B368">
+        <v>0.92553898632090226</v>
+      </c>
+      <c r="C368">
+        <v>0.96924972534179688</v>
+      </c>
+      <c r="D368">
+        <v>0.96869683265686035</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>28.610861509846579</v>
+      </c>
+      <c r="B369">
+        <v>0.90347052698609642</v>
+      </c>
+      <c r="C369">
+        <v>0.93569344282150269</v>
+      </c>
+      <c r="D369">
+        <v>0.93888479471206665</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>27.942182534555521</v>
+      </c>
+      <c r="B370">
+        <v>0.94486284382727714</v>
+      </c>
+      <c r="C370">
+        <v>0.94640392065048218</v>
+      </c>
+      <c r="D370">
+        <v>0.95346271991729736</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>30.409894530846348</v>
+      </c>
+      <c r="B371">
+        <v>0.94031141656620809</v>
+      </c>
+      <c r="C371">
+        <v>0.97776752710342407</v>
+      </c>
+      <c r="D371">
+        <v>0.9790617823600769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>